<commit_message>
Minimal working prototype of edit trooper
</commit_message>
<xml_diff>
--- a/trial/Normal Week of 190824.xlsx
+++ b/trial/Normal Week of 190824.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
-  <si>
-    <t>DUTY 230824 FRIDAY</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+  <si>
+    <t>DUTY 250824 SUNDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -64,10 +64,13 @@
     <t>SENTRY</t>
   </si>
   <si>
+    <t>IN</t>
+  </si>
+  <si>
     <t>X-RAY</t>
   </si>
   <si>
-    <t>IN</t>
+    <t>DESK</t>
   </si>
   <si>
     <t>JIAN JUN</t>
@@ -79,42 +82,42 @@
     <t>KAH FAI</t>
   </si>
   <si>
+    <t>DI ER</t>
+  </si>
+  <si>
+    <t>SCA1</t>
+  </si>
+  <si>
+    <t>XAVIER</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>ANIQ</t>
+  </si>
+  <si>
+    <t>JUN</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>SYAFI'I</t>
+  </si>
+  <si>
+    <t>JOSHUA</t>
+  </si>
+  <si>
+    <t>ANIISH</t>
+  </si>
+  <si>
+    <t>HILMI</t>
+  </si>
+  <si>
     <t>SCA2</t>
   </si>
   <si>
-    <t>DI ER</t>
-  </si>
-  <si>
-    <t>SCA1</t>
-  </si>
-  <si>
-    <t>XAVIER</t>
-  </si>
-  <si>
-    <t>DESK</t>
-  </si>
-  <si>
-    <t>ANIQ</t>
-  </si>
-  <si>
-    <t>JUN</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>SYAFI'I</t>
-  </si>
-  <si>
-    <t>JOSHUA</t>
-  </si>
-  <si>
-    <t>ANIISH</t>
-  </si>
-  <si>
-    <t>HILMI</t>
-  </si>
-  <si>
     <t>HUGO</t>
   </si>
   <si>
@@ -124,16 +127,13 @@
     <t>MARC</t>
   </si>
   <si>
-    <t>PAC</t>
-  </si>
-  <si>
-    <t>FLAG:MARC // DI ER // KAH FAI</t>
-  </si>
-  <si>
-    <t>LAST ENSURER: KAH FAI</t>
-  </si>
-  <si>
-    <t>BREAKFAST:ANIQ // DINNER:HAKIM</t>
+    <t>FLAG:MARC // KAH FAI // XAVIER</t>
+  </si>
+  <si>
+    <t>LAST ENSURER: DI ER</t>
+  </si>
+  <si>
+    <t>BREAKFAST:MARC // DINNER:ANIQ</t>
   </si>
 </sst>
 </file>
@@ -200,13 +200,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,19 +224,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
+        <fgColor rgb="FFF4CCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,31 +276,31 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -675,23 +675,25 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="4">
         <v>6</v>
@@ -703,26 +705,26 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="4">
@@ -735,26 +737,26 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="6" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="7"/>
       <c r="N7" s="4">
         <v>6</v>
       </c>
@@ -767,24 +769,24 @@
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="5"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
       <c r="N9" s="4">
         <v>6</v>
       </c>
@@ -797,24 +799,28 @@
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="10" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="10"/>
+      <c r="M11" s="11"/>
       <c r="N11" s="4">
         <v>6</v>
       </c>
@@ -827,28 +833,26 @@
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="4"/>
       <c r="N13" s="4">
         <v>6</v>
       </c>
@@ -861,20 +865,20 @@
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
       <c r="N15" s="4">
         <v>0</v>
       </c>
@@ -887,20 +891,20 @@
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
       <c r="N17" s="4">
         <v>0</v>
       </c>
@@ -913,28 +917,28 @@
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="7" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="9"/>
       <c r="N19" s="4">
         <v>6</v>
       </c>
@@ -947,20 +951,20 @@
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
       <c r="N21" s="4">
         <v>0</v>
       </c>
@@ -973,28 +977,26 @@
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="8" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="7" t="s">
+      <c r="J23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="M23" s="6"/>
       <c r="N23" s="4">
         <v>6</v>
       </c>
@@ -1005,30 +1007,30 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="H25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
       <c r="N25" s="4">
         <v>6</v>
       </c>
@@ -1039,30 +1041,30 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="K27" s="8" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M27" s="7"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
       <c r="N27" s="4">
         <v>6</v>
       </c>
@@ -1073,28 +1075,30 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L29" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="M29" s="12"/>
+      <c r="E29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="8"/>
+      <c r="K29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
       <c r="N29" s="4">
         <v>6</v>
       </c>
@@ -1154,27 +1158,26 @@
       <c r="N32" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="L7:M7"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="B15:M15"/>
     <mergeCell ref="B17:M17"/>
     <mergeCell ref="L19:M19"/>
     <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="L23:M23"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="L29:M29"/>
     <mergeCell ref="A30:C32"/>
     <mergeCell ref="K30:N32"/>
     <mergeCell ref="D30:J32"/>

</xml_diff>

<commit_message>
Fixed minor bugs (part 1?) before rolling out first prototype
</commit_message>
<xml_diff>
--- a/trial/Normal Week of 190824.xlsx
+++ b/trial/Normal Week of 190824.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>DUTY 250824 SUNDAY</t>
   </si>
@@ -67,40 +67,43 @@
     <t>IN</t>
   </si>
   <si>
+    <t>JIAN JUN</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>KAH FAI</t>
+  </si>
+  <si>
+    <t>DI ER</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>XAVIER</t>
+  </si>
+  <si>
     <t>X-RAY</t>
   </si>
   <si>
     <t>DESK</t>
   </si>
   <si>
-    <t>JIAN JUN</t>
-  </si>
-  <si>
-    <t>OUT</t>
-  </si>
-  <si>
-    <t>KAH FAI</t>
-  </si>
-  <si>
-    <t>DI ER</t>
+    <t>ANIQ</t>
   </si>
   <si>
     <t>SCA1</t>
   </si>
   <si>
-    <t>XAVIER</t>
-  </si>
-  <si>
-    <t>PAC</t>
-  </si>
-  <si>
-    <t>ANIQ</t>
-  </si>
-  <si>
     <t>JUN</t>
   </si>
   <si>
-    <t>MC</t>
+    <t>SCA2</t>
+  </si>
+  <si>
+    <t>ANIISH</t>
   </si>
   <si>
     <t>SYAFI'I</t>
@@ -109,15 +112,9 @@
     <t>JOSHUA</t>
   </si>
   <si>
-    <t>ANIISH</t>
-  </si>
-  <si>
     <t>HILMI</t>
   </si>
   <si>
-    <t>SCA2</t>
-  </si>
-  <si>
     <t>HUGO</t>
   </si>
   <si>
@@ -127,13 +124,13 @@
     <t>MARC</t>
   </si>
   <si>
-    <t>FLAG:MARC // KAH FAI // XAVIER</t>
-  </si>
-  <si>
-    <t>LAST ENSURER: DI ER</t>
-  </si>
-  <si>
-    <t>BREAKFAST:MARC // DINNER:ANIQ</t>
+    <t>FLAG:KAH FAI // HUGO // HAKIM</t>
+  </si>
+  <si>
+    <t>LAST ENSURER: ANIQ</t>
+  </si>
+  <si>
+    <t>BREAKFAST:ANIISH // DINNER:KAH FAI</t>
   </si>
 </sst>
 </file>
@@ -173,7 +170,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +203,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -219,18 +222,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF999999"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,12 +273,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,10 +288,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -683,20 +671,16 @@
       <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -705,22 +689,20 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>18</v>
+      <c r="J5" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>15</v>
@@ -728,7 +710,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -737,28 +719,26 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="7"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="6"/>
       <c r="N7" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -767,28 +747,26 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="M9" s="8"/>
       <c r="N9" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -797,32 +775,30 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="11"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
       <c r="N11" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -831,30 +807,30 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="9" t="s">
+      <c r="J13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="4"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
       <c r="N13" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -865,22 +841,26 @@
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
       <c r="N15" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -891,22 +871,28 @@
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
       <c r="N17" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -917,30 +903,28 @@
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="4"/>
       <c r="N19" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -951,22 +935,28 @@
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="10"/>
       <c r="N21" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -977,28 +967,26 @@
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="8"/>
-      <c r="L23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M23" s="6"/>
+      <c r="B23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
       <c r="N23" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1007,32 +995,30 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="E25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="F25" s="7"/>
       <c r="G25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
       <c r="N25" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1041,32 +1027,30 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B27" s="7"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="K27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="9"/>
       <c r="N27" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1075,108 +1059,103 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="13" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="19">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="E7:G7"/>
     <mergeCell ref="L7:M7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B21:M21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="L27:M27"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="A30:C32"/>
     <mergeCell ref="K30:N32"/>

</xml_diff>